<commit_message>
removed tracking of AP
</commit_message>
<xml_diff>
--- a/DnD information-0.11.xlsx
+++ b/DnD information-0.11.xlsx
@@ -695,6 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -719,7 +720,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1246,7 +1246,7 @@
       <c r="E14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="32" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="32" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1524,16 +1524,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
       <c r="K2" s="14" t="s">
         <v>51</v>
       </c>
@@ -1555,10 +1555,10 @@
       <c r="G3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="32"/>
+      <c r="I3" s="33"/>
       <c r="K3" s="15" t="s">
         <v>52</v>
       </c>
@@ -1572,8 +1572,8 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
       <c r="K4" s="16" t="s">
         <v>53</v>
       </c>
@@ -1658,24 +1658,24 @@
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="18" t="s">
         <v>55</v>
       </c>

</xml_diff>